<commit_message>
feat: FINISH DOCS SPECS
</commit_message>
<xml_diff>
--- a/planning/StellaStone - Planning.xlsx
+++ b/planning/StellaStone - Planning.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7600A73F-9461-4DA5-9718-635474C14774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20140FD0-1D72-4803-B9F2-E825E37001EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -793,7 +793,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1006,17 +1006,6 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="0" tint="-0.14993743705557422"/>
       </left>
       <right/>
@@ -1031,48 +1020,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color theme="0" tint="-0.14993743705557422"/>
-      </right>
-      <top style="medium">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC00000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFC00000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFC00000"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC00000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFC00000"/>
       </right>
       <top style="medium">
         <color theme="0" tint="-0.14996795556505021"/>
@@ -1154,7 +1102,7 @@
     <xf numFmtId="0" fontId="7" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1337,24 +1285,6 @@
     <xf numFmtId="0" fontId="0" fillId="47" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="5" fillId="48" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1400,59 +1330,68 @@
     <xf numFmtId="167" fontId="7" fillId="51" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="49" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="49" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="51" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="51" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="46" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="46" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="49" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="49" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="51" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="51" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="46" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="46" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1511,7 +1450,31 @@
     <cellStyle name="Vérification" xfId="25" builtinId="23" customBuiltin="1"/>
     <cellStyle name="zTexteMasqué" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1728,15 +1691,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ListeTâches" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="totalRow" dxfId="18"/>
-      <tableStyleElement type="firstColumn" dxfId="17"/>
-      <tableStyleElement type="lastColumn" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="22"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="totalRow" dxfId="20"/>
+      <tableStyleElement type="firstColumn" dxfId="19"/>
+      <tableStyleElement type="lastColumn" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="17"/>
+      <tableStyleElement type="secondRowStripe" dxfId="16"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="15"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="14"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2156,7 +2119,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z9" sqref="Z9"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2207,116 +2170,116 @@
         <v>4</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="93">
+      <c r="D3" s="97"/>
+      <c r="E3" s="99">
         <v>44851</v>
       </c>
-      <c r="F3" s="93"/>
+      <c r="F3" s="99"/>
     </row>
     <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="88"/>
+      <c r="D4" s="97"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="89">
+      <c r="I4" s="84">
         <f>I5</f>
         <v>44851</v>
       </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="89">
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="84">
         <f>P5</f>
         <v>44858</v>
       </c>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="89">
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="84">
         <f>W5</f>
         <v>44865</v>
       </c>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="89">
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
+      <c r="Z4" s="85"/>
+      <c r="AA4" s="85"/>
+      <c r="AB4" s="85"/>
+      <c r="AC4" s="86"/>
+      <c r="AD4" s="84">
         <f>AD5</f>
         <v>44872</v>
       </c>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="90"/>
-      <c r="AG4" s="90"/>
-      <c r="AH4" s="90"/>
-      <c r="AI4" s="90"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="89">
+      <c r="AE4" s="85"/>
+      <c r="AF4" s="85"/>
+      <c r="AG4" s="85"/>
+      <c r="AH4" s="85"/>
+      <c r="AI4" s="85"/>
+      <c r="AJ4" s="86"/>
+      <c r="AK4" s="84">
         <f>AK5</f>
         <v>44879</v>
       </c>
-      <c r="AL4" s="90"/>
-      <c r="AM4" s="90"/>
-      <c r="AN4" s="90"/>
-      <c r="AO4" s="90"/>
-      <c r="AP4" s="90"/>
-      <c r="AQ4" s="91"/>
-      <c r="AR4" s="89">
+      <c r="AL4" s="85"/>
+      <c r="AM4" s="85"/>
+      <c r="AN4" s="85"/>
+      <c r="AO4" s="85"/>
+      <c r="AP4" s="85"/>
+      <c r="AQ4" s="86"/>
+      <c r="AR4" s="84">
         <f>AR5</f>
         <v>44886</v>
       </c>
-      <c r="AS4" s="90"/>
-      <c r="AT4" s="90"/>
-      <c r="AU4" s="90"/>
-      <c r="AV4" s="90"/>
-      <c r="AW4" s="90"/>
-      <c r="AX4" s="91"/>
-      <c r="AY4" s="89">
+      <c r="AS4" s="85"/>
+      <c r="AT4" s="85"/>
+      <c r="AU4" s="85"/>
+      <c r="AV4" s="85"/>
+      <c r="AW4" s="85"/>
+      <c r="AX4" s="86"/>
+      <c r="AY4" s="84">
         <f>AY5</f>
         <v>44893</v>
       </c>
-      <c r="AZ4" s="90"/>
-      <c r="BA4" s="90"/>
-      <c r="BB4" s="90"/>
-      <c r="BC4" s="90"/>
-      <c r="BD4" s="90"/>
-      <c r="BE4" s="91"/>
-      <c r="BF4" s="89">
+      <c r="AZ4" s="85"/>
+      <c r="BA4" s="85"/>
+      <c r="BB4" s="85"/>
+      <c r="BC4" s="85"/>
+      <c r="BD4" s="85"/>
+      <c r="BE4" s="86"/>
+      <c r="BF4" s="84">
         <f>BF5</f>
         <v>44900</v>
       </c>
-      <c r="BG4" s="90"/>
-      <c r="BH4" s="90"/>
-      <c r="BI4" s="90"/>
-      <c r="BJ4" s="90"/>
-      <c r="BK4" s="90"/>
-      <c r="BL4" s="91"/>
-      <c r="BM4" s="89">
+      <c r="BG4" s="85"/>
+      <c r="BH4" s="85"/>
+      <c r="BI4" s="85"/>
+      <c r="BJ4" s="85"/>
+      <c r="BK4" s="85"/>
+      <c r="BL4" s="86"/>
+      <c r="BM4" s="84">
         <f>BM5</f>
         <v>44907</v>
       </c>
-      <c r="BN4" s="90"/>
-      <c r="BO4" s="90"/>
-      <c r="BP4" s="90"/>
-      <c r="BQ4" s="90"/>
-      <c r="BR4" s="90"/>
-      <c r="BS4" s="91"/>
+      <c r="BN4" s="85"/>
+      <c r="BO4" s="85"/>
+      <c r="BP4" s="85"/>
+      <c r="BQ4" s="85"/>
+      <c r="BR4" s="85"/>
+      <c r="BS4" s="86"/>
     </row>
     <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
@@ -2585,10 +2548,10 @@
       <c r="A6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="92" t="s">
+      <c r="B6" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="92"/>
+      <c r="C6" s="98"/>
       <c r="D6" s="7" t="s">
         <v>11</v>
       </c>
@@ -2802,15 +2765,15 @@
         <f t="shared" si="9"/>
         <v>l</v>
       </c>
-      <c r="BG6" s="66" t="str">
+      <c r="BG6" s="8" t="str">
         <f t="shared" si="9"/>
         <v>m</v>
       </c>
-      <c r="BH6" s="70" t="str">
+      <c r="BH6" s="8" t="str">
         <f t="shared" si="9"/>
         <v>m</v>
       </c>
-      <c r="BI6" s="68" t="str">
+      <c r="BI6" s="8" t="str">
         <f t="shared" si="9"/>
         <v>j</v>
       </c>
@@ -2914,12 +2877,12 @@
       <c r="BC7" s="17"/>
       <c r="BD7" s="17"/>
       <c r="BE7" s="17"/>
-      <c r="BF7" s="17"/>
-      <c r="BG7" s="67"/>
-      <c r="BH7" s="71"/>
-      <c r="BI7" s="69"/>
-      <c r="BJ7" s="17"/>
-      <c r="BK7" s="17"/>
+      <c r="BF7" s="81"/>
+      <c r="BG7" s="100"/>
+      <c r="BH7" s="81"/>
+      <c r="BI7" s="101"/>
+      <c r="BJ7" s="81"/>
+      <c r="BK7" s="81"/>
       <c r="BL7" s="17"/>
       <c r="BM7" s="65"/>
       <c r="BN7" s="65"/>
@@ -2994,12 +2957,12 @@
       <c r="BC8" s="17"/>
       <c r="BD8" s="17"/>
       <c r="BE8" s="17"/>
-      <c r="BF8" s="17"/>
-      <c r="BG8" s="67"/>
-      <c r="BH8" s="71"/>
-      <c r="BI8" s="69"/>
-      <c r="BJ8" s="17"/>
-      <c r="BK8" s="17"/>
+      <c r="BF8" s="81"/>
+      <c r="BG8" s="100"/>
+      <c r="BH8" s="81"/>
+      <c r="BI8" s="101"/>
+      <c r="BJ8" s="81"/>
+      <c r="BK8" s="81"/>
       <c r="BL8" s="17"/>
       <c r="BM8" s="65"/>
       <c r="BN8" s="65"/>
@@ -3013,12 +2976,12 @@
       <c r="A9" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="100" t="s">
+      <c r="B9" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="100"/>
+      <c r="C9" s="91"/>
       <c r="D9" s="12">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E9" s="44">
         <v>44844</v>
@@ -3080,12 +3043,12 @@
       <c r="BC9" s="17"/>
       <c r="BD9" s="17"/>
       <c r="BE9" s="17"/>
-      <c r="BF9" s="17"/>
-      <c r="BG9" s="67"/>
-      <c r="BH9" s="71"/>
-      <c r="BI9" s="69"/>
-      <c r="BJ9" s="17"/>
-      <c r="BK9" s="17"/>
+      <c r="BF9" s="81"/>
+      <c r="BG9" s="100"/>
+      <c r="BH9" s="81"/>
+      <c r="BI9" s="101"/>
+      <c r="BJ9" s="81"/>
+      <c r="BK9" s="81"/>
       <c r="BL9" s="17"/>
       <c r="BM9" s="65"/>
       <c r="BN9" s="65"/>
@@ -3095,7 +3058,7 @@
       <c r="BR9" s="17"/>
       <c r="BS9" s="17"/>
     </row>
-    <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>16</v>
       </c>
@@ -3160,12 +3123,12 @@
       <c r="BC10" s="17"/>
       <c r="BD10" s="17"/>
       <c r="BE10" s="17"/>
-      <c r="BF10" s="17"/>
-      <c r="BG10" s="67"/>
-      <c r="BH10" s="71"/>
-      <c r="BI10" s="69"/>
-      <c r="BJ10" s="17"/>
-      <c r="BK10" s="17"/>
+      <c r="BF10" s="81"/>
+      <c r="BG10" s="100"/>
+      <c r="BH10" s="81"/>
+      <c r="BI10" s="101"/>
+      <c r="BJ10" s="81"/>
+      <c r="BK10" s="81"/>
       <c r="BL10" s="17"/>
       <c r="BM10" s="65"/>
       <c r="BN10" s="65"/>
@@ -3175,16 +3138,16 @@
       <c r="BR10" s="17"/>
       <c r="BS10" s="17"/>
     </row>
-    <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="100" t="s">
+      <c r="B11" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="100"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="12">
-        <v>0.25</v>
+        <v>0.83</v>
       </c>
       <c r="E11" s="44">
         <v>44858</v>
@@ -3246,12 +3209,12 @@
       <c r="BC11" s="17"/>
       <c r="BD11" s="17"/>
       <c r="BE11" s="17"/>
-      <c r="BF11" s="17"/>
-      <c r="BG11" s="67"/>
-      <c r="BH11" s="71"/>
-      <c r="BI11" s="69"/>
-      <c r="BJ11" s="17"/>
-      <c r="BK11" s="17"/>
+      <c r="BF11" s="81"/>
+      <c r="BG11" s="100"/>
+      <c r="BH11" s="81"/>
+      <c r="BI11" s="101"/>
+      <c r="BJ11" s="81"/>
+      <c r="BK11" s="81"/>
       <c r="BL11" s="17"/>
       <c r="BM11" s="65"/>
       <c r="BN11" s="65"/>
@@ -3261,7 +3224,7 @@
       <c r="BR11" s="17"/>
       <c r="BS11" s="17"/>
     </row>
-    <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
         <v>21</v>
       </c>
@@ -3326,12 +3289,12 @@
       <c r="BC12" s="17"/>
       <c r="BD12" s="17"/>
       <c r="BE12" s="17"/>
-      <c r="BF12" s="17"/>
-      <c r="BG12" s="67"/>
-      <c r="BH12" s="71"/>
-      <c r="BI12" s="69"/>
-      <c r="BJ12" s="17"/>
-      <c r="BK12" s="17"/>
+      <c r="BF12" s="81"/>
+      <c r="BG12" s="100"/>
+      <c r="BH12" s="81"/>
+      <c r="BI12" s="101"/>
+      <c r="BJ12" s="81"/>
+      <c r="BK12" s="81"/>
       <c r="BL12" s="17"/>
       <c r="BM12" s="65"/>
       <c r="BN12" s="65"/>
@@ -3341,25 +3304,25 @@
       <c r="BR12" s="17"/>
       <c r="BS12" s="17"/>
     </row>
-    <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30"/>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="102"/>
+      <c r="C13" s="93"/>
       <c r="D13" s="14">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="E13" s="47">
         <v>44876</v>
       </c>
       <c r="F13" s="47">
-        <v>44900</v>
+        <v>44905</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
@@ -3410,12 +3373,12 @@
       <c r="BC13" s="17"/>
       <c r="BD13" s="17"/>
       <c r="BE13" s="17"/>
-      <c r="BF13" s="17"/>
-      <c r="BG13" s="67"/>
-      <c r="BH13" s="71"/>
-      <c r="BI13" s="69"/>
-      <c r="BJ13" s="17"/>
-      <c r="BK13" s="17"/>
+      <c r="BF13" s="81"/>
+      <c r="BG13" s="100"/>
+      <c r="BH13" s="81"/>
+      <c r="BI13" s="101"/>
+      <c r="BJ13" s="81"/>
+      <c r="BK13" s="81"/>
       <c r="BL13" s="17"/>
       <c r="BM13" s="65"/>
       <c r="BN13" s="65"/>
@@ -3425,7 +3388,7 @@
       <c r="BR13" s="17"/>
       <c r="BS13" s="17"/>
     </row>
-    <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>24</v>
       </c>
@@ -3490,12 +3453,12 @@
       <c r="BC14" s="17"/>
       <c r="BD14" s="17"/>
       <c r="BE14" s="17"/>
-      <c r="BF14" s="17"/>
-      <c r="BG14" s="67"/>
-      <c r="BH14" s="71"/>
-      <c r="BI14" s="69"/>
-      <c r="BJ14" s="17"/>
-      <c r="BK14" s="17"/>
+      <c r="BF14" s="81"/>
+      <c r="BG14" s="100"/>
+      <c r="BH14" s="81"/>
+      <c r="BI14" s="101"/>
+      <c r="BJ14" s="81"/>
+      <c r="BK14" s="81"/>
       <c r="BL14" s="17"/>
       <c r="BM14" s="65"/>
       <c r="BN14" s="65"/>
@@ -3505,12 +3468,12 @@
       <c r="BR14" s="17"/>
       <c r="BS14" s="17"/>
     </row>
-    <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="99"/>
+      <c r="C15" s="90"/>
       <c r="D15" s="16">
         <v>0</v>
       </c>
@@ -3518,12 +3481,12 @@
         <v>44883</v>
       </c>
       <c r="F15" s="50">
-        <v>44901</v>
+        <v>44909</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10">
         <f t="shared" si="10"/>
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
@@ -3574,12 +3537,12 @@
       <c r="BC15" s="17"/>
       <c r="BD15" s="17"/>
       <c r="BE15" s="17"/>
-      <c r="BF15" s="17"/>
-      <c r="BG15" s="67"/>
-      <c r="BH15" s="71"/>
-      <c r="BI15" s="69"/>
-      <c r="BJ15" s="17"/>
-      <c r="BK15" s="17"/>
+      <c r="BF15" s="81"/>
+      <c r="BG15" s="100"/>
+      <c r="BH15" s="81"/>
+      <c r="BI15" s="101"/>
+      <c r="BJ15" s="81"/>
+      <c r="BK15" s="81"/>
       <c r="BL15" s="17"/>
       <c r="BM15" s="65"/>
       <c r="BN15" s="65"/>
@@ -3589,7 +3552,7 @@
       <c r="BR15" s="17"/>
       <c r="BS15" s="17"/>
     </row>
-    <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>24</v>
       </c>
@@ -3654,12 +3617,12 @@
       <c r="BC16" s="17"/>
       <c r="BD16" s="17"/>
       <c r="BE16" s="17"/>
-      <c r="BF16" s="17"/>
-      <c r="BG16" s="67"/>
-      <c r="BH16" s="71"/>
-      <c r="BI16" s="69"/>
-      <c r="BJ16" s="17"/>
-      <c r="BK16" s="17"/>
+      <c r="BF16" s="81"/>
+      <c r="BG16" s="100"/>
+      <c r="BH16" s="81"/>
+      <c r="BI16" s="101"/>
+      <c r="BJ16" s="81"/>
+      <c r="BK16" s="81"/>
       <c r="BL16" s="17"/>
       <c r="BM16" s="65"/>
       <c r="BN16" s="65"/>
@@ -3669,26 +3632,26 @@
       <c r="BR16" s="17"/>
       <c r="BS16" s="17"/>
     </row>
-    <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="99"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="16">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E17" s="50">
         <v>44890</v>
       </c>
       <c r="F17" s="50">
-        <f>E17+11</f>
-        <v>44901</v>
+        <f>E17+17</f>
+        <v>44907</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
@@ -3739,12 +3702,12 @@
       <c r="BC17" s="17"/>
       <c r="BD17" s="17"/>
       <c r="BE17" s="17"/>
-      <c r="BF17" s="17"/>
-      <c r="BG17" s="67"/>
-      <c r="BH17" s="71"/>
-      <c r="BI17" s="69"/>
-      <c r="BJ17" s="17"/>
-      <c r="BK17" s="17"/>
+      <c r="BF17" s="81"/>
+      <c r="BG17" s="100"/>
+      <c r="BH17" s="81"/>
+      <c r="BI17" s="101"/>
+      <c r="BJ17" s="81"/>
+      <c r="BK17" s="81"/>
       <c r="BL17" s="17"/>
       <c r="BM17" s="65"/>
       <c r="BN17" s="65"/>
@@ -3754,7 +3717,7 @@
       <c r="BR17" s="17"/>
       <c r="BS17" s="17"/>
     </row>
-    <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>24</v>
       </c>
@@ -3819,12 +3782,12 @@
       <c r="BC18" s="17"/>
       <c r="BD18" s="17"/>
       <c r="BE18" s="17"/>
-      <c r="BF18" s="17"/>
-      <c r="BG18" s="67"/>
-      <c r="BH18" s="71"/>
-      <c r="BI18" s="69"/>
-      <c r="BJ18" s="17"/>
-      <c r="BK18" s="17"/>
+      <c r="BF18" s="81"/>
+      <c r="BG18" s="100"/>
+      <c r="BH18" s="81"/>
+      <c r="BI18" s="101"/>
+      <c r="BJ18" s="81"/>
+      <c r="BK18" s="81"/>
       <c r="BL18" s="17"/>
       <c r="BM18" s="65"/>
       <c r="BN18" s="65"/>
@@ -3834,14 +3797,14 @@
       <c r="BR18" s="17"/>
       <c r="BS18" s="17"/>
     </row>
-    <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="99"/>
+      <c r="C19" s="90"/>
       <c r="D19" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="50">
         <v>44876</v>
@@ -3903,12 +3866,12 @@
       <c r="BC19" s="17"/>
       <c r="BD19" s="17"/>
       <c r="BE19" s="17"/>
-      <c r="BF19" s="17"/>
-      <c r="BG19" s="67"/>
-      <c r="BH19" s="71"/>
-      <c r="BI19" s="69"/>
-      <c r="BJ19" s="17"/>
-      <c r="BK19" s="17"/>
+      <c r="BF19" s="81"/>
+      <c r="BG19" s="100"/>
+      <c r="BH19" s="81"/>
+      <c r="BI19" s="101"/>
+      <c r="BJ19" s="81"/>
+      <c r="BK19" s="81"/>
       <c r="BL19" s="17"/>
       <c r="BM19" s="65"/>
       <c r="BN19" s="65"/>
@@ -3918,17 +3881,17 @@
       <c r="BR19" s="17"/>
       <c r="BS19" s="17"/>
     </row>
-    <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="76"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10" t="str">
         <f t="shared" si="10"/>
@@ -3983,12 +3946,12 @@
       <c r="BC20" s="17"/>
       <c r="BD20" s="17"/>
       <c r="BE20" s="17"/>
-      <c r="BF20" s="17"/>
-      <c r="BG20" s="67"/>
-      <c r="BH20" s="71"/>
-      <c r="BI20" s="69"/>
-      <c r="BJ20" s="17"/>
-      <c r="BK20" s="17"/>
+      <c r="BF20" s="81"/>
+      <c r="BG20" s="100"/>
+      <c r="BH20" s="81"/>
+      <c r="BI20" s="101"/>
+      <c r="BJ20" s="81"/>
+      <c r="BK20" s="81"/>
       <c r="BL20" s="17"/>
       <c r="BM20" s="65"/>
       <c r="BN20" s="65"/>
@@ -3998,27 +3961,27 @@
       <c r="BR20" s="17"/>
       <c r="BS20" s="17"/>
     </row>
-    <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="95"/>
-      <c r="D21" s="78">
-        <v>0</v>
-      </c>
-      <c r="E21" s="79">
+      <c r="C21" s="83"/>
+      <c r="D21" s="72">
+        <v>0.25</v>
+      </c>
+      <c r="E21" s="73">
         <v>44890</v>
       </c>
-      <c r="F21" s="79">
-        <v>44902</v>
+      <c r="F21" s="73">
+        <v>44905</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
@@ -4069,12 +4032,12 @@
       <c r="BC21" s="17"/>
       <c r="BD21" s="17"/>
       <c r="BE21" s="17"/>
-      <c r="BF21" s="17"/>
-      <c r="BG21" s="67"/>
-      <c r="BH21" s="71"/>
-      <c r="BI21" s="69"/>
-      <c r="BJ21" s="17"/>
-      <c r="BK21" s="17"/>
+      <c r="BF21" s="81"/>
+      <c r="BG21" s="100"/>
+      <c r="BH21" s="81"/>
+      <c r="BI21" s="101"/>
+      <c r="BJ21" s="81"/>
+      <c r="BK21" s="81"/>
       <c r="BL21" s="17"/>
       <c r="BM21" s="65"/>
       <c r="BN21" s="65"/>
@@ -4084,14 +4047,14 @@
       <c r="BR21" s="17"/>
       <c r="BS21" s="17"/>
     </row>
-    <row r="22" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="77" t="s">
+    <row r="22" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="76"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="70"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10" t="str">
         <f t="shared" si="10"/>
@@ -4146,12 +4109,12 @@
       <c r="BC22" s="17"/>
       <c r="BD22" s="17"/>
       <c r="BE22" s="17"/>
-      <c r="BF22" s="17"/>
-      <c r="BG22" s="67"/>
-      <c r="BH22" s="71"/>
-      <c r="BI22" s="69"/>
-      <c r="BJ22" s="17"/>
-      <c r="BK22" s="17"/>
+      <c r="BF22" s="81"/>
+      <c r="BG22" s="100"/>
+      <c r="BH22" s="81"/>
+      <c r="BI22" s="101"/>
+      <c r="BJ22" s="81"/>
+      <c r="BK22" s="81"/>
       <c r="BL22" s="17"/>
       <c r="BM22" s="65"/>
       <c r="BN22" s="65"/>
@@ -4161,24 +4124,24 @@
       <c r="BR22" s="17"/>
       <c r="BS22" s="17"/>
     </row>
-    <row r="23" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="94" t="s">
+    <row r="23" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="95"/>
-      <c r="D23" s="78">
-        <v>0</v>
-      </c>
-      <c r="E23" s="79">
+      <c r="C23" s="83"/>
+      <c r="D23" s="72">
+        <v>0.3</v>
+      </c>
+      <c r="E23" s="73">
         <v>44902</v>
       </c>
-      <c r="F23" s="79">
-        <v>44906</v>
+      <c r="F23" s="73">
+        <v>44911</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
@@ -4229,12 +4192,12 @@
       <c r="BC23" s="17"/>
       <c r="BD23" s="17"/>
       <c r="BE23" s="17"/>
-      <c r="BF23" s="17"/>
-      <c r="BG23" s="67"/>
-      <c r="BH23" s="71"/>
-      <c r="BI23" s="69"/>
-      <c r="BJ23" s="17"/>
-      <c r="BK23" s="17"/>
+      <c r="BF23" s="81"/>
+      <c r="BG23" s="100"/>
+      <c r="BH23" s="81"/>
+      <c r="BI23" s="101"/>
+      <c r="BJ23" s="81"/>
+      <c r="BK23" s="81"/>
       <c r="BL23" s="17"/>
       <c r="BM23" s="65"/>
       <c r="BN23" s="65"/>
@@ -4244,7 +4207,7 @@
       <c r="BR23" s="17"/>
       <c r="BS23" s="17"/>
     </row>
-    <row r="24" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="63" t="s">
         <v>33</v>
       </c>
@@ -4303,12 +4266,12 @@
       <c r="BC24" s="17"/>
       <c r="BD24" s="17"/>
       <c r="BE24" s="17"/>
-      <c r="BF24" s="17"/>
-      <c r="BG24" s="67"/>
-      <c r="BH24" s="71"/>
-      <c r="BI24" s="69"/>
-      <c r="BJ24" s="17"/>
-      <c r="BK24" s="17"/>
+      <c r="BF24" s="81"/>
+      <c r="BG24" s="100"/>
+      <c r="BH24" s="81"/>
+      <c r="BI24" s="101"/>
+      <c r="BJ24" s="81"/>
+      <c r="BK24" s="81"/>
       <c r="BL24" s="17"/>
       <c r="BM24" s="65"/>
       <c r="BN24" s="65"/>
@@ -4318,11 +4281,11 @@
       <c r="BR24" s="17"/>
       <c r="BS24" s="17"/>
     </row>
-    <row r="25" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="103" t="s">
+    <row r="25" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="104"/>
+      <c r="C25" s="95"/>
       <c r="D25" s="61">
         <v>0</v>
       </c>
@@ -4386,12 +4349,12 @@
       <c r="BC25" s="17"/>
       <c r="BD25" s="17"/>
       <c r="BE25" s="17"/>
-      <c r="BF25" s="17"/>
-      <c r="BG25" s="67"/>
-      <c r="BH25" s="71"/>
-      <c r="BI25" s="69"/>
-      <c r="BJ25" s="17"/>
-      <c r="BK25" s="17"/>
+      <c r="BF25" s="81"/>
+      <c r="BG25" s="100"/>
+      <c r="BH25" s="81"/>
+      <c r="BI25" s="101"/>
+      <c r="BJ25" s="81"/>
+      <c r="BK25" s="81"/>
       <c r="BL25" s="17"/>
       <c r="BM25" s="65"/>
       <c r="BN25" s="65"/>
@@ -4401,14 +4364,14 @@
       <c r="BR25" s="17"/>
       <c r="BS25" s="17"/>
     </row>
-    <row r="26" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="80" t="s">
+    <row r="26" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="81"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="84"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="78"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="17"/>
@@ -4460,12 +4423,12 @@
       <c r="BC26" s="17"/>
       <c r="BD26" s="17"/>
       <c r="BE26" s="17"/>
-      <c r="BF26" s="17"/>
-      <c r="BG26" s="67"/>
-      <c r="BH26" s="71"/>
-      <c r="BI26" s="69"/>
-      <c r="BJ26" s="17"/>
-      <c r="BK26" s="17"/>
+      <c r="BF26" s="81"/>
+      <c r="BG26" s="100"/>
+      <c r="BH26" s="81"/>
+      <c r="BI26" s="101"/>
+      <c r="BJ26" s="81"/>
+      <c r="BK26" s="81"/>
       <c r="BL26" s="17"/>
       <c r="BM26" s="65"/>
       <c r="BN26" s="65"/>
@@ -4475,18 +4438,18 @@
       <c r="BR26" s="17"/>
       <c r="BS26" s="17"/>
     </row>
-    <row r="27" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="96" t="s">
+    <row r="27" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="97"/>
-      <c r="D27" s="85">
+      <c r="C27" s="88"/>
+      <c r="D27" s="79">
         <v>0</v>
       </c>
-      <c r="E27" s="86">
+      <c r="E27" s="80">
         <v>44907</v>
       </c>
-      <c r="F27" s="86">
+      <c r="F27" s="80">
         <v>44911</v>
       </c>
       <c r="G27" s="10"/>
@@ -4543,12 +4506,12 @@
       <c r="BC27" s="17"/>
       <c r="BD27" s="17"/>
       <c r="BE27" s="17"/>
-      <c r="BF27" s="17"/>
-      <c r="BG27" s="67"/>
-      <c r="BH27" s="71"/>
-      <c r="BI27" s="69"/>
-      <c r="BJ27" s="17"/>
-      <c r="BK27" s="17"/>
+      <c r="BF27" s="81"/>
+      <c r="BG27" s="100"/>
+      <c r="BH27" s="81"/>
+      <c r="BI27" s="101"/>
+      <c r="BJ27" s="81"/>
+      <c r="BK27" s="81"/>
       <c r="BL27" s="17"/>
       <c r="BM27" s="65"/>
       <c r="BN27" s="65"/>
@@ -4563,6 +4526,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="BM4:BS4"/>
     <mergeCell ref="B21:C21"/>
@@ -4579,16 +4549,9 @@
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D27">
-    <cfRule type="dataBar" priority="23">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4601,56 +4564,66 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL21">
-    <cfRule type="expression" dxfId="11" priority="42">
+  <conditionalFormatting sqref="I5:BL5 I7:BG21 BL6 BI7:BL21 BH7:BH27 I6:BJ6">
+    <cfRule type="expression" dxfId="13" priority="44">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL21">
-    <cfRule type="expression" dxfId="10" priority="36">
+  <conditionalFormatting sqref="I7:BG21 BI7:BL21 BH7:BH27">
+    <cfRule type="expression" dxfId="12" priority="38">
       <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="39" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22:BL27">
-    <cfRule type="expression" dxfId="8" priority="9">
+  <conditionalFormatting sqref="I22:BG27 BI22:BL27">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22:BL27">
-    <cfRule type="expression" dxfId="7" priority="7">
+  <conditionalFormatting sqref="I22:BG27 BI22:BL27">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM5:BS21">
-    <cfRule type="expression" dxfId="5" priority="6">
+  <conditionalFormatting sqref="BM5:BS5 BM7:BS21 BS6">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM7:BS21">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>AND(début_tâche&lt;=BM$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=BM$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=BM$5,début_tâche&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM22:BS27">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM22:BS27">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>AND(début_tâche&lt;=BM$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=BM$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=BM$5,début_tâche&lt;BN$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM6:BR6">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BK6">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(TODAY()&gt;=BK$5,TODAY()&lt;BL$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4817,15 +4790,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5113,6 +5077,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
   <ds:schemaRefs>
@@ -5126,14 +5099,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5152,4 +5117,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>